<commit_message>
Modification 2 first notebook (integrate computing with the github files)
</commit_message>
<xml_diff>
--- a/Medium_Glu_Cit_AC_doe3.xlsx
+++ b/Medium_Glu_Cit_AC_doe3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Desktop\Master Thesis\Master\Mile2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70137615-F71B-4F76-86AE-07B61B18AD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571C5DFC-DC88-4365-B9C7-8765490CD9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
   <si>
     <t>Sample</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>0_196_2D.csv</t>
+  </si>
+  <si>
+    <t>23A_53_2D.csv</t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B394" sqref="B394"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="B361" sqref="B361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10718,7 +10721,7 @@
     </row>
     <row r="362" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="31" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B362" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10744,7 +10747,7 @@
     <row r="363" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="31" t="str">
         <f t="shared" ref="A363:A376" si="24">TEXT(LEFT(A362,3),"00A")&amp;"_"&amp;TEXT(MID(A362,5,2)+1,"00")&amp;"_2D.csv"</f>
-        <v>23A_53_2D.csv</v>
+        <v>23A_54_2D.csv</v>
       </c>
       <c r="B363" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10770,7 +10773,7 @@
     <row r="364" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_54_2D.csv</v>
+        <v>23A_55_2D.csv</v>
       </c>
       <c r="B364" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10796,7 +10799,7 @@
     <row r="365" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_55_2D.csv</v>
+        <v>23A_56_2D.csv</v>
       </c>
       <c r="B365" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10822,7 +10825,7 @@
     <row r="366" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_56_2D.csv</v>
+        <v>23A_57_2D.csv</v>
       </c>
       <c r="B366" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10848,7 +10851,7 @@
     <row r="367" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_57_2D.csv</v>
+        <v>23A_58_2D.csv</v>
       </c>
       <c r="B367" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10874,7 +10877,7 @@
     <row r="368" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_58_2D.csv</v>
+        <v>23A_59_2D.csv</v>
       </c>
       <c r="B368" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10900,7 +10903,7 @@
     <row r="369" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_59_2D.csv</v>
+        <v>23A_60_2D.csv</v>
       </c>
       <c r="B369" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10926,7 +10929,7 @@
     <row r="370" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_60_2D.csv</v>
+        <v>23A_61_2D.csv</v>
       </c>
       <c r="B370" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10952,7 +10955,7 @@
     <row r="371" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_61_2D.csv</v>
+        <v>23A_62_2D.csv</v>
       </c>
       <c r="B371" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -10978,7 +10981,7 @@
     <row r="372" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_62_2D.csv</v>
+        <v>23A_63_2D.csv</v>
       </c>
       <c r="B372" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -11004,7 +11007,7 @@
     <row r="373" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_63_2D.csv</v>
+        <v>23A_64_2D.csv</v>
       </c>
       <c r="B373" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -11030,7 +11033,7 @@
     <row r="374" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_64_2D.csv</v>
+        <v>23A_65_2D.csv</v>
       </c>
       <c r="B374" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -11056,7 +11059,7 @@
     <row r="375" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_65_2D.csv</v>
+        <v>23A_66_2D.csv</v>
       </c>
       <c r="B375" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -11082,7 +11085,7 @@
     <row r="376" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>23A_66_2D.csv</v>
+        <v>23A_67_2D.csv</v>
       </c>
       <c r="B376" s="1" t="str">
         <f>Samples!$A$32</f>
@@ -15855,7 +15858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q25" sqref="Q25"/>
     </sheetView>

</xml_diff>